<commit_message>
Implemented r-skript for mca baeume
</commit_message>
<xml_diff>
--- a/00_data_raw/Belaege_Gewichtung_Szenario0.xlsx
+++ b/00_data_raw/Belaege_Gewichtung_Szenario0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/pfeifsar_students_zhaw_ch/Documents/6. Semester MSc UnR/Thesis/R_Project/00_data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{72486D78-DEF3-48B5-ABEC-3983F2E8BA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA559FFC-5619-4BD1-849A-56EFDDDEE068}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{72486D78-DEF3-48B5-ABEC-3983F2E8BA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1ABC4B1-02F1-4650-A073-30352AD27F91}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="-1350" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21765" yWindow="225" windowWidth="19125" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gewichtung" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>group_id</t>
   </si>
@@ -96,9 +96,6 @@
     <t>befahrbarkeit</t>
   </si>
   <si>
-    <t>barrierefreiheit</t>
-  </si>
-  <si>
     <t>recyclingfaehigkeit</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
   </si>
   <si>
     <t>Befahrbarkeit</t>
-  </si>
-  <si>
-    <t>Barrierefreiheit</t>
   </si>
   <si>
     <t>Recyclingfähigkeit</t>
@@ -234,6 +228,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -523,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -573,7 +571,7 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2">
         <v>0.5</v>
@@ -590,10 +588,10 @@
         <v>0.1</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3">
         <v>0.5</v>
@@ -604,7 +602,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>0.4</v>
@@ -613,7 +611,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4">
         <v>0.5</v>
@@ -624,7 +622,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>0.4</v>
@@ -633,7 +631,7 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>0.25</v>
@@ -644,7 +642,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>0.4</v>
@@ -653,7 +651,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6">
         <v>0.25</v>
@@ -673,10 +671,11 @@
         <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7">
-        <v>0.25</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -693,10 +692,11 @@
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8">
-        <v>0.25</v>
+        <f t="shared" ref="F8:F9" si="0">1/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -713,30 +713,32 @@
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9">
-        <v>0.25</v>
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10">
-        <v>0.25</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -750,13 +752,13 @@
         <v>0.1</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11">
-        <f>1/3</f>
+        <f t="shared" ref="F11:F12" si="1">1/3</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -771,34 +773,13 @@
         <v>0.1</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:F13" si="0">1/3</f>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13">
-        <v>0.1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -822,7 +803,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>